<commit_message>
update doc test plan
</commit_message>
<xml_diff>
--- a/ScenarioTestDocs_MOBILE-12072022.xlsx
+++ b/ScenarioTestDocs_MOBILE-12072022.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="85">
   <si>
     <t>Created By</t>
   </si>
@@ -482,6 +482,30 @@
   <si>
     <t>You did not confirm your password correctly</t>
   </si>
+  <si>
+    <t>Verify login with registered user</t>
+  </si>
+  <si>
+    <t>Verify login with unregistered user</t>
+  </si>
+  <si>
+    <t>2.  input username, password</t>
+  </si>
+  <si>
+    <t>3. Tap login</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> username = sum4                           password = sum4                 </t>
+  </si>
+  <si>
+    <t>redirect to dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> username = sum4 1324                          password = sum434                </t>
+  </si>
+  <si>
+    <t>Incorrect username or password</t>
+  </si>
 </sst>
 </file>
 
@@ -573,7 +597,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="48">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -922,19 +946,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color rgb="FF000000"/>
@@ -1140,7 +1151,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="128">
+  <cellXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1217,285 +1228,270 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1712,10 +1708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB1009"/>
+  <dimension ref="A1:AB1003"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="94" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="94" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1736,20 +1732,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="56" t="s">
+      <c r="A1" s="99" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
+      <c r="B1" s="88"/>
       <c r="C1" s="1" t="s">
         <v>46</v>
       </c>
       <c r="D1" s="2"/>
-      <c r="E1" s="56" t="s">
+      <c r="E1" s="99" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="49"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="54"/>
+      <c r="F1" s="88"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="86"/>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
@@ -1802,22 +1798,22 @@
       <c r="AB2" s="3"/>
     </row>
     <row r="3" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="87" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="49"/>
+      <c r="B3" s="88"/>
       <c r="C3" s="1" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="2"/>
-      <c r="E3" s="48" t="s">
+      <c r="E3" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="49"/>
-      <c r="G3" s="61">
+      <c r="F3" s="88"/>
+      <c r="G3" s="90">
         <v>44741</v>
       </c>
-      <c r="H3" s="54"/>
+      <c r="H3" s="86"/>
       <c r="I3" s="4"/>
       <c r="J3" s="4"/>
       <c r="K3" s="4"/>
@@ -1870,15 +1866,15 @@
       <c r="AB4" s="3"/>
     </row>
     <row r="5" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="89" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="49"/>
+      <c r="B5" s="88"/>
       <c r="C5" s="6" t="s">
         <v>46</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="53" t="s">
+      <c r="E5" s="116" t="s">
         <v>5</v>
       </c>
       <c r="F5" s="7" t="s">
@@ -1916,7 +1912,7 @@
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="47"/>
+      <c r="E6" s="71"/>
       <c r="F6" s="10">
         <v>8</v>
       </c>
@@ -1978,29 +1974,29 @@
       <c r="AB7" s="3"/>
     </row>
     <row r="8" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="77" t="s">
+      <c r="A8" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="88" t="s">
+      <c r="C8" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="92" t="s">
+      <c r="D8" s="117" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="93"/>
-      <c r="F8" s="89" t="s">
+      <c r="E8" s="118"/>
+      <c r="F8" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="74" t="s">
+      <c r="G8" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="75" t="s">
+      <c r="H8" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="I8" s="76" t="s">
+      <c r="I8" s="36" t="s">
         <v>16</v>
       </c>
       <c r="J8" s="2"/>
@@ -2024,27 +2020,27 @@
       <c r="AB8" s="3"/>
     </row>
     <row r="9" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="99" t="s">
+      <c r="A9" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="99" t="s">
+      <c r="B9" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="105" t="s">
+      <c r="C9" s="93" t="s">
         <v>63</v>
       </c>
-      <c r="D9" s="107" t="s">
+      <c r="D9" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="E9" s="108"/>
-      <c r="F9" s="72"/>
-      <c r="G9" s="116" t="s">
+      <c r="E9" s="64"/>
+      <c r="F9" s="32"/>
+      <c r="G9" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="H9" s="116" t="s">
+      <c r="H9" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="123"/>
+      <c r="I9" s="53"/>
       <c r="J9" s="2"/>
       <c r="K9" s="12"/>
       <c r="L9" s="12"/>
@@ -2066,21 +2062,21 @@
       <c r="AB9" s="3"/>
     </row>
     <row r="10" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="82"/>
-      <c r="B10" s="102"/>
-      <c r="C10" s="85"/>
-      <c r="D10" s="109" t="s">
+      <c r="A10" s="61"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="94"/>
+      <c r="D10" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="E10" s="110"/>
-      <c r="F10" s="72"/>
-      <c r="G10" s="117" t="s">
+      <c r="E10" s="66"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="H10" s="117" t="s">
+      <c r="H10" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="I10" s="123"/>
+      <c r="I10" s="53"/>
       <c r="J10" s="2"/>
       <c r="K10" s="12"/>
       <c r="L10" s="12"/>
@@ -2102,19 +2098,19 @@
       <c r="AB10" s="3"/>
     </row>
     <row r="11" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="82"/>
-      <c r="B11" s="102"/>
-      <c r="C11" s="85"/>
-      <c r="D11" s="109" t="s">
+      <c r="A11" s="61"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="94"/>
+      <c r="D11" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="110"/>
-      <c r="F11" s="95" t="s">
+      <c r="E11" s="66"/>
+      <c r="F11" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="118"/>
-      <c r="H11" s="121"/>
-      <c r="I11" s="123"/>
+      <c r="G11" s="50"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="53"/>
       <c r="J11" s="2"/>
       <c r="K11" s="12"/>
       <c r="L11" s="12"/>
@@ -2136,21 +2132,21 @@
       <c r="AB11" s="3"/>
     </row>
     <row r="12" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="83"/>
-      <c r="B12" s="102"/>
-      <c r="C12" s="86"/>
-      <c r="D12" s="111" t="s">
+      <c r="A12" s="62"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="95"/>
+      <c r="D12" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="E12" s="112"/>
-      <c r="F12" s="87"/>
-      <c r="G12" s="119" t="s">
+      <c r="E12" s="68"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="H12" s="119" t="s">
+      <c r="H12" s="51" t="s">
         <v>72</v>
       </c>
-      <c r="I12" s="124" t="s">
+      <c r="I12" s="54" t="s">
         <v>73</v>
       </c>
       <c r="J12" s="2"/>
@@ -2174,25 +2170,25 @@
       <c r="AB12" s="3"/>
     </row>
     <row r="13" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="99" t="s">
+      <c r="A13" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="102"/>
-      <c r="C13" s="106" t="s">
+      <c r="B13" s="58"/>
+      <c r="C13" s="60" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="107" t="s">
+      <c r="D13" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="E13" s="108"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="116" t="s">
+      <c r="E13" s="64"/>
+      <c r="F13" s="32"/>
+      <c r="G13" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="H13" s="116" t="s">
+      <c r="H13" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="I13" s="123"/>
+      <c r="I13" s="53"/>
       <c r="J13" s="2"/>
       <c r="K13" s="12"/>
       <c r="L13" s="12"/>
@@ -2214,21 +2210,21 @@
       <c r="AB13" s="3"/>
     </row>
     <row r="14" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="82"/>
-      <c r="B14" s="102"/>
-      <c r="C14" s="82"/>
-      <c r="D14" s="109" t="s">
+      <c r="A14" s="61"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="E14" s="110"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="117" t="s">
+      <c r="E14" s="66"/>
+      <c r="F14" s="32"/>
+      <c r="G14" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="H14" s="117" t="s">
+      <c r="H14" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="I14" s="123"/>
+      <c r="I14" s="53"/>
       <c r="J14" s="2"/>
       <c r="K14" s="12"/>
       <c r="L14" s="12"/>
@@ -2250,19 +2246,19 @@
       <c r="AB14" s="3"/>
     </row>
     <row r="15" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="82"/>
-      <c r="B15" s="102"/>
-      <c r="C15" s="82"/>
-      <c r="D15" s="109" t="s">
+      <c r="A15" s="61"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="110"/>
-      <c r="F15" s="95" t="s">
+      <c r="E15" s="66"/>
+      <c r="F15" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="G15" s="118"/>
-      <c r="H15" s="121"/>
-      <c r="I15" s="123"/>
+      <c r="G15" s="50"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="53"/>
       <c r="J15" s="2"/>
       <c r="K15" s="12"/>
       <c r="L15" s="12"/>
@@ -2284,21 +2280,21 @@
       <c r="AB15" s="3"/>
     </row>
     <row r="16" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="83"/>
-      <c r="B16" s="102"/>
-      <c r="C16" s="83"/>
-      <c r="D16" s="111" t="s">
+      <c r="A16" s="62"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="E16" s="112"/>
-      <c r="F16" s="104"/>
-      <c r="G16" s="119" t="s">
+      <c r="E16" s="68"/>
+      <c r="F16" s="47"/>
+      <c r="G16" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="H16" s="119" t="s">
+      <c r="H16" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="124" t="s">
+      <c r="I16" s="54" t="s">
         <v>73</v>
       </c>
       <c r="J16" s="2"/>
@@ -2322,25 +2318,25 @@
       <c r="AB16" s="3"/>
     </row>
     <row r="17" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="99" t="s">
+      <c r="A17" s="57" t="s">
         <v>18</v>
       </c>
-      <c r="B17" s="102"/>
-      <c r="C17" s="106" t="s">
+      <c r="B17" s="58"/>
+      <c r="C17" s="60" t="s">
         <v>65</v>
       </c>
-      <c r="D17" s="107" t="s">
+      <c r="D17" s="63" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="108"/>
-      <c r="F17" s="72"/>
-      <c r="G17" s="116" t="s">
+      <c r="E17" s="64"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="H17" s="116" t="s">
+      <c r="H17" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="123"/>
+      <c r="I17" s="53"/>
       <c r="J17" s="2"/>
       <c r="K17" s="12"/>
       <c r="L17" s="12"/>
@@ -2362,21 +2358,21 @@
       <c r="AB17" s="3"/>
     </row>
     <row r="18" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="82"/>
-      <c r="B18" s="102"/>
-      <c r="C18" s="82"/>
-      <c r="D18" s="109" t="s">
+      <c r="A18" s="61"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="110"/>
-      <c r="F18" s="72"/>
-      <c r="G18" s="117" t="s">
+      <c r="E18" s="66"/>
+      <c r="F18" s="32"/>
+      <c r="G18" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="H18" s="117" t="s">
+      <c r="H18" s="49" t="s">
         <v>70</v>
       </c>
-      <c r="I18" s="123"/>
+      <c r="I18" s="53"/>
       <c r="J18" s="2"/>
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
@@ -2398,19 +2394,19 @@
       <c r="AB18" s="3"/>
     </row>
     <row r="19" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="82"/>
-      <c r="B19" s="102"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="109" t="s">
+      <c r="A19" s="61"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="61"/>
+      <c r="D19" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="110"/>
-      <c r="F19" s="95" t="s">
+      <c r="E19" s="66"/>
+      <c r="F19" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="G19" s="118"/>
-      <c r="H19" s="121"/>
-      <c r="I19" s="123"/>
+      <c r="G19" s="50"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="53"/>
       <c r="J19" s="2"/>
       <c r="K19" s="12"/>
       <c r="L19" s="12"/>
@@ -2432,21 +2428,21 @@
       <c r="AB19" s="3"/>
     </row>
     <row r="20" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="83"/>
-      <c r="B20" s="103"/>
-      <c r="C20" s="83"/>
-      <c r="D20" s="111" t="s">
+      <c r="A20" s="62"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="67" t="s">
         <v>68</v>
       </c>
-      <c r="E20" s="112"/>
-      <c r="F20" s="87"/>
-      <c r="G20" s="119" t="s">
+      <c r="E20" s="68"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="51" t="s">
         <v>76</v>
       </c>
-      <c r="H20" s="126" t="s">
+      <c r="H20" s="55" t="s">
         <v>76</v>
       </c>
-      <c r="I20" s="127" t="s">
+      <c r="I20" s="56" t="s">
         <v>73</v>
       </c>
       <c r="J20" s="2"/>
@@ -2470,19 +2466,27 @@
       <c r="AB20" s="3"/>
     </row>
     <row r="21" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="99" t="s">
+      <c r="A21" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="99" t="s">
+      <c r="B21" s="57" t="s">
         <v>61</v>
       </c>
-      <c r="C21" s="81"/>
-      <c r="D21" s="113"/>
-      <c r="E21" s="114"/>
-      <c r="F21" s="72"/>
-      <c r="G21" s="118"/>
-      <c r="H21" s="121"/>
-      <c r="I21" s="123"/>
+      <c r="C21" s="60" t="s">
+        <v>77</v>
+      </c>
+      <c r="D21" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E21" s="64"/>
+      <c r="F21" s="121"/>
+      <c r="G21" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="H21" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="I21" s="53"/>
       <c r="J21" s="2"/>
       <c r="K21" s="12"/>
       <c r="L21" s="12"/>
@@ -2504,15 +2508,19 @@
       <c r="AB21" s="3"/>
     </row>
     <row r="22" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="82"/>
-      <c r="B22" s="102"/>
-      <c r="C22" s="82"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="110"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="118"/>
-      <c r="H22" s="121"/>
-      <c r="I22" s="123"/>
+      <c r="A22" s="61"/>
+      <c r="B22" s="58"/>
+      <c r="C22" s="61"/>
+      <c r="D22" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="E22" s="66"/>
+      <c r="F22" s="44" t="s">
+        <v>81</v>
+      </c>
+      <c r="G22" s="50"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="53"/>
       <c r="J22" s="2"/>
       <c r="K22" s="12"/>
       <c r="L22" s="12"/>
@@ -2534,15 +2542,23 @@
       <c r="AB22" s="3"/>
     </row>
     <row r="23" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="82"/>
-      <c r="B23" s="102"/>
-      <c r="C23" s="82"/>
-      <c r="D23" s="109"/>
-      <c r="E23" s="110"/>
-      <c r="F23" s="72"/>
-      <c r="G23" s="118"/>
-      <c r="H23" s="121"/>
-      <c r="I23" s="123"/>
+      <c r="A23" s="61"/>
+      <c r="B23" s="58"/>
+      <c r="C23" s="61"/>
+      <c r="D23" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="68"/>
+      <c r="F23" s="122"/>
+      <c r="G23" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="H23" s="51" t="s">
+        <v>82</v>
+      </c>
+      <c r="I23" s="56" t="s">
+        <v>73</v>
+      </c>
       <c r="J23" s="2"/>
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
@@ -2564,15 +2580,25 @@
       <c r="AB23" s="3"/>
     </row>
     <row r="24" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="83"/>
-      <c r="B24" s="102"/>
-      <c r="C24" s="83"/>
-      <c r="D24" s="111"/>
-      <c r="E24" s="112"/>
-      <c r="F24" s="87"/>
-      <c r="G24" s="120"/>
-      <c r="H24" s="122"/>
-      <c r="I24" s="125"/>
+      <c r="A24" s="57" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="58"/>
+      <c r="C24" s="60" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="63" t="s">
+        <v>49</v>
+      </c>
+      <c r="E24" s="64"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="H24" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="I24" s="53"/>
       <c r="J24" s="2"/>
       <c r="K24" s="12"/>
       <c r="L24" s="12"/>
@@ -2594,17 +2620,19 @@
       <c r="AB24" s="3"/>
     </row>
     <row r="25" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="99" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="102"/>
-      <c r="C25" s="81"/>
-      <c r="D25" s="109"/>
-      <c r="E25" s="110"/>
-      <c r="F25" s="72"/>
-      <c r="G25" s="118"/>
-      <c r="H25" s="121"/>
-      <c r="I25" s="123"/>
+      <c r="A25" s="61"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="61"/>
+      <c r="D25" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="E25" s="66"/>
+      <c r="F25" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="G25" s="50"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="53"/>
       <c r="J25" s="2"/>
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
@@ -2626,15 +2654,23 @@
       <c r="AB25" s="3"/>
     </row>
     <row r="26" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="82"/>
-      <c r="B26" s="102"/>
-      <c r="C26" s="82"/>
-      <c r="D26" s="109"/>
-      <c r="E26" s="110"/>
-      <c r="F26" s="72"/>
-      <c r="G26" s="118"/>
-      <c r="H26" s="121"/>
-      <c r="I26" s="123"/>
+      <c r="A26" s="61"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="61"/>
+      <c r="D26" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="68"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="H26" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="I26" s="56" t="s">
+        <v>73</v>
+      </c>
       <c r="J26" s="2"/>
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
@@ -2655,19 +2691,31 @@
       <c r="AA26" s="3"/>
       <c r="AB26" s="3"/>
     </row>
-    <row r="27" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="82"/>
-      <c r="B27" s="102"/>
-      <c r="C27" s="82"/>
-      <c r="D27" s="109"/>
-      <c r="E27" s="110"/>
-      <c r="F27" s="72"/>
-      <c r="G27" s="118"/>
-      <c r="H27" s="121"/>
-      <c r="I27" s="123"/>
+    <row r="27" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="110" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" s="101" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="72" t="s">
+        <v>62</v>
+      </c>
+      <c r="D27" s="91" t="s">
+        <v>49</v>
+      </c>
+      <c r="E27" s="92"/>
+      <c r="F27" s="43"/>
+      <c r="G27" s="46" t="s">
+        <v>53</v>
+      </c>
+      <c r="H27" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" s="39"/>
       <c r="J27" s="2"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
       <c r="M27" s="2"/>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
@@ -2685,19 +2733,25 @@
       <c r="AA27" s="3"/>
       <c r="AB27" s="3"/>
     </row>
-    <row r="28" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="83"/>
+    <row r="28" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="111"/>
       <c r="B28" s="102"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="111"/>
-      <c r="E28" s="112"/>
-      <c r="F28" s="87"/>
-      <c r="G28" s="120"/>
-      <c r="H28" s="122"/>
-      <c r="I28" s="125"/>
+      <c r="C28" s="113"/>
+      <c r="D28" s="76" t="s">
+        <v>50</v>
+      </c>
+      <c r="E28" s="96"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="29" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I28" s="29"/>
       <c r="J28" s="2"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="4"/>
       <c r="M28" s="2"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
@@ -2715,21 +2769,21 @@
       <c r="AA28" s="3"/>
       <c r="AB28" s="3"/>
     </row>
-    <row r="29" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="99" t="s">
-        <v>21</v>
-      </c>
+    <row r="29" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="111"/>
       <c r="B29" s="102"/>
-      <c r="C29" s="84"/>
-      <c r="D29" s="109"/>
-      <c r="E29" s="110"/>
-      <c r="F29" s="72"/>
-      <c r="G29" s="118"/>
-      <c r="H29" s="121"/>
-      <c r="I29" s="123"/>
+      <c r="C29" s="113"/>
+      <c r="D29" s="103" t="s">
+        <v>51</v>
+      </c>
+      <c r="E29" s="104"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="16"/>
+      <c r="I29" s="29"/>
       <c r="J29" s="2"/>
-      <c r="K29" s="12"/>
-      <c r="L29" s="12"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
       <c r="M29" s="2"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
@@ -2747,19 +2801,29 @@
       <c r="AA29" s="3"/>
       <c r="AB29" s="3"/>
     </row>
-    <row r="30" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="82"/>
+    <row r="30" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="112"/>
       <c r="B30" s="102"/>
-      <c r="C30" s="85"/>
-      <c r="D30" s="109"/>
-      <c r="E30" s="110"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="118"/>
-      <c r="H30" s="121"/>
-      <c r="I30" s="123"/>
+      <c r="C30" s="114"/>
+      <c r="D30" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="E30" s="106"/>
+      <c r="F30" s="45" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" s="30" t="s">
+        <v>56</v>
+      </c>
+      <c r="H30" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="I30" s="30" t="s">
+        <v>6</v>
+      </c>
       <c r="J30" s="2"/>
-      <c r="K30" s="12"/>
-      <c r="L30" s="12"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="4"/>
       <c r="M30" s="2"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
@@ -2777,19 +2841,29 @@
       <c r="AA30" s="3"/>
       <c r="AB30" s="3"/>
     </row>
-    <row r="31" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="82"/>
+    <row r="31" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="97" t="s">
+        <v>18</v>
+      </c>
       <c r="B31" s="102"/>
-      <c r="C31" s="85"/>
-      <c r="D31" s="109"/>
-      <c r="E31" s="110"/>
-      <c r="F31" s="72"/>
-      <c r="G31" s="118"/>
-      <c r="H31" s="121"/>
-      <c r="I31" s="123"/>
-      <c r="J31" s="2"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
+      <c r="C31" s="72" t="s">
+        <v>57</v>
+      </c>
+      <c r="D31" s="107" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="108"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="H31" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="I31" s="29"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="4"/>
       <c r="M31" s="2"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
@@ -2807,19 +2881,25 @@
       <c r="AA31" s="3"/>
       <c r="AB31" s="3"/>
     </row>
-    <row r="32" spans="1:28" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="83"/>
-      <c r="B32" s="103"/>
-      <c r="C32" s="86"/>
-      <c r="D32" s="111"/>
-      <c r="E32" s="112"/>
-      <c r="F32" s="72"/>
-      <c r="G32" s="118"/>
-      <c r="H32" s="121"/>
-      <c r="I32" s="123"/>
-      <c r="J32" s="2"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
+    <row r="32" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="73"/>
+      <c r="B32" s="102"/>
+      <c r="C32" s="73"/>
+      <c r="D32" s="76" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="100"/>
+      <c r="F32" s="13"/>
+      <c r="G32" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H32" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="I32" s="29"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="4"/>
       <c r="M32" s="2"/>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
@@ -2837,32 +2917,24 @@
       <c r="AA32" s="3"/>
       <c r="AB32" s="3"/>
     </row>
-    <row r="33" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="98" t="s">
-        <v>17</v>
-      </c>
-      <c r="B33" s="57" t="s">
-        <v>48</v>
-      </c>
-      <c r="C33" s="28" t="s">
-        <v>62</v>
-      </c>
-      <c r="D33" s="78" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" s="90"/>
-      <c r="F33" s="94"/>
-      <c r="G33" s="97" t="s">
-        <v>53</v>
-      </c>
-      <c r="H33" s="79" t="s">
-        <v>54</v>
-      </c>
-      <c r="I33" s="80"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="4"/>
-      <c r="M33" s="2"/>
+    <row r="33" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="73"/>
+      <c r="B33" s="102"/>
+      <c r="C33" s="73"/>
+      <c r="D33" s="103" t="s">
+        <v>51</v>
+      </c>
+      <c r="E33" s="109"/>
+      <c r="F33" s="20" t="s">
+        <v>58</v>
+      </c>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+      <c r="M33" s="3"/>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
       <c r="P33" s="3"/>
@@ -2879,26 +2951,28 @@
       <c r="AA33" s="3"/>
       <c r="AB33" s="3"/>
     </row>
-    <row r="34" spans="1:28" ht="16.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="100"/>
-      <c r="B34" s="58"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="E34" s="33"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="H34" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="I34" s="66"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="4"/>
-      <c r="L34" s="4"/>
-      <c r="M34" s="2"/>
+    <row r="34" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="98"/>
+      <c r="B34" s="102"/>
+      <c r="C34" s="98"/>
+      <c r="D34" s="105" t="s">
+        <v>69</v>
+      </c>
+      <c r="E34" s="115"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="H34" s="28" t="s">
+        <v>59</v>
+      </c>
+      <c r="I34" s="30" t="s">
+        <v>6</v>
+      </c>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="3"/>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
       <c r="P34" s="3"/>
@@ -2915,22 +2989,30 @@
       <c r="AA34" s="3"/>
       <c r="AB34" s="3"/>
     </row>
-    <row r="35" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="100"/>
-      <c r="B35" s="58"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="E35" s="91"/>
-      <c r="F35" s="95"/>
-      <c r="G35" s="66"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="66"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="2"/>
+    <row r="35" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="69" t="s">
+        <v>19</v>
+      </c>
+      <c r="B35" s="82" t="s">
+        <v>60</v>
+      </c>
+      <c r="C35" s="72" t="s">
+        <v>44</v>
+      </c>
+      <c r="D35" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="E35" s="77"/>
+      <c r="F35" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G35" s="20"/>
+      <c r="H35" s="20"/>
+      <c r="I35" s="15"/>
+      <c r="J35" s="3"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+      <c r="M35" s="3"/>
       <c r="N35" s="3"/>
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
@@ -2947,30 +3029,24 @@
       <c r="AA35" s="3"/>
       <c r="AB35" s="3"/>
     </row>
-    <row r="36" spans="1:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="101"/>
-      <c r="B36" s="58"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="115" t="s">
-        <v>69</v>
-      </c>
-      <c r="E36" s="69"/>
-      <c r="F36" s="96" t="s">
-        <v>52</v>
-      </c>
-      <c r="G36" s="67" t="s">
-        <v>56</v>
-      </c>
-      <c r="H36" s="18" t="s">
-        <v>56</v>
-      </c>
-      <c r="I36" s="67" t="s">
-        <v>6</v>
-      </c>
-      <c r="J36" s="2"/>
-      <c r="K36" s="4"/>
-      <c r="L36" s="4"/>
-      <c r="M36" s="2"/>
+    <row r="36" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="70"/>
+      <c r="B36" s="83"/>
+      <c r="C36" s="73"/>
+      <c r="D36" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="E36" s="77"/>
+      <c r="F36" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="G36" s="20"/>
+      <c r="H36" s="20"/>
+      <c r="I36" s="15"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="3"/>
       <c r="N36" s="3"/>
       <c r="O36" s="3"/>
       <c r="P36" s="3"/>
@@ -2988,29 +3064,23 @@
       <c r="AB36" s="3"/>
     </row>
     <row r="37" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="55" t="s">
-        <v>18</v>
-      </c>
-      <c r="B37" s="58"/>
-      <c r="C37" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="D37" s="62" t="s">
-        <v>49</v>
-      </c>
-      <c r="E37" s="71"/>
-      <c r="F37" s="13"/>
-      <c r="G37" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="H37" s="64" t="s">
-        <v>54</v>
-      </c>
-      <c r="I37" s="66"/>
-      <c r="J37" s="4"/>
-      <c r="K37" s="4"/>
-      <c r="L37" s="4"/>
-      <c r="M37" s="2"/>
+      <c r="A37" s="70"/>
+      <c r="B37" s="83"/>
+      <c r="C37" s="74"/>
+      <c r="D37" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="E37" s="77"/>
+      <c r="F37" s="21">
+        <v>44742</v>
+      </c>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="15"/>
+      <c r="J37" s="3"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+      <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
@@ -3027,26 +3097,24 @@
       <c r="AA37" s="3"/>
       <c r="AB37" s="3"/>
     </row>
-    <row r="38" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="51"/>
-      <c r="B38" s="58"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="31" t="s">
-        <v>50</v>
-      </c>
-      <c r="E38" s="32"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="H38" s="16" t="s">
-        <v>55</v>
-      </c>
-      <c r="I38" s="66"/>
-      <c r="J38" s="4"/>
-      <c r="K38" s="4"/>
-      <c r="L38" s="4"/>
-      <c r="M38" s="2"/>
+    <row r="38" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="70"/>
+      <c r="B38" s="83"/>
+      <c r="C38" s="74"/>
+      <c r="D38" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" s="78"/>
+      <c r="F38" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="15"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
@@ -3063,21 +3131,25 @@
       <c r="AA38" s="3"/>
       <c r="AB38" s="3"/>
     </row>
-    <row r="39" spans="1:28" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="51"/>
-      <c r="B39" s="58"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="45" t="s">
-        <v>51</v>
-      </c>
-      <c r="E39" s="70"/>
-      <c r="F39" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="G39" s="16"/>
-      <c r="H39" s="16"/>
-      <c r="I39" s="66"/>
-      <c r="J39" s="4"/>
+    <row r="39" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="71"/>
+      <c r="B39" s="83"/>
+      <c r="C39" s="75"/>
+      <c r="D39" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="E39" s="80"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H39" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I39" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="J39" s="3"/>
       <c r="K39" s="3"/>
       <c r="L39" s="3"/>
       <c r="M39" s="3"/>
@@ -3098,23 +3170,23 @@
       <c r="AB39" s="3"/>
     </row>
     <row r="40" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="52"/>
-      <c r="B40" s="58"/>
-      <c r="C40" s="52"/>
-      <c r="D40" s="115" t="s">
-        <v>69</v>
-      </c>
-      <c r="E40" s="50"/>
-      <c r="F40" s="17"/>
-      <c r="G40" s="63" t="s">
-        <v>59</v>
-      </c>
-      <c r="H40" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="I40" s="67" t="s">
-        <v>6</v>
-      </c>
+      <c r="A40" s="69" t="s">
+        <v>20</v>
+      </c>
+      <c r="B40" s="83"/>
+      <c r="C40" s="81" t="s">
+        <v>43</v>
+      </c>
+      <c r="D40" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="77"/>
+      <c r="F40" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" s="20"/>
+      <c r="H40" s="20"/>
+      <c r="I40" s="15"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
@@ -3136,21 +3208,15 @@
       <c r="AB40" s="3"/>
     </row>
     <row r="41" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="26" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="36" t="s">
-        <v>60</v>
-      </c>
-      <c r="C41" s="28" t="s">
-        <v>44</v>
-      </c>
-      <c r="D41" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E41" s="42"/>
+      <c r="A41" s="70"/>
+      <c r="B41" s="83"/>
+      <c r="C41" s="74"/>
+      <c r="D41" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="E41" s="77"/>
       <c r="F41" s="20" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G41" s="20"/>
       <c r="H41" s="20"/>
@@ -3176,18 +3242,18 @@
       <c r="AB41" s="3"/>
     </row>
     <row r="42" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="46"/>
-      <c r="B42" s="37"/>
-      <c r="C42" s="51"/>
-      <c r="D42" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E42" s="42"/>
-      <c r="F42" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
+      <c r="A42" s="70"/>
+      <c r="B42" s="83"/>
+      <c r="C42" s="74"/>
+      <c r="D42" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="77"/>
+      <c r="F42" s="21">
+        <v>36703</v>
+      </c>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
       <c r="I42" s="15"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -3210,15 +3276,15 @@
       <c r="AB42" s="3"/>
     </row>
     <row r="43" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="46"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E43" s="42"/>
-      <c r="F43" s="21">
-        <v>44742</v>
+      <c r="A43" s="70"/>
+      <c r="B43" s="83"/>
+      <c r="C43" s="74"/>
+      <c r="D43" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="E43" s="78"/>
+      <c r="F43" s="23" t="s">
+        <v>13</v>
       </c>
       <c r="G43" s="21"/>
       <c r="H43" s="21"/>
@@ -3244,19 +3310,23 @@
       <c r="AB43" s="3"/>
     </row>
     <row r="44" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="46"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E44" s="43"/>
-      <c r="F44" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G44" s="21"/>
-      <c r="H44" s="21"/>
-      <c r="I44" s="15"/>
+      <c r="A44" s="71"/>
+      <c r="B44" s="83"/>
+      <c r="C44" s="75"/>
+      <c r="D44" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="E44" s="80"/>
+      <c r="F44" s="24"/>
+      <c r="G44" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="H44" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I44" s="25" t="s">
+        <v>7</v>
+      </c>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
       <c r="L44" s="3"/>
@@ -3278,23 +3348,23 @@
       <c r="AB44" s="3"/>
     </row>
     <row r="45" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="47"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="41"/>
-      <c r="D45" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E45" s="44"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H45" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I45" s="19" t="s">
-        <v>6</v>
-      </c>
+      <c r="A45" s="69" t="s">
+        <v>21</v>
+      </c>
+      <c r="B45" s="83"/>
+      <c r="C45" s="72" t="s">
+        <v>45</v>
+      </c>
+      <c r="D45" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="E45" s="77"/>
+      <c r="F45" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="G45" s="20"/>
+      <c r="H45" s="20"/>
+      <c r="I45" s="15"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
       <c r="L45" s="3"/>
@@ -3316,19 +3386,15 @@
       <c r="AB45" s="3"/>
     </row>
     <row r="46" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B46" s="37"/>
-      <c r="C46" s="39" t="s">
-        <v>43</v>
-      </c>
-      <c r="D46" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E46" s="42"/>
+      <c r="A46" s="70"/>
+      <c r="B46" s="83"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="77"/>
       <c r="F46" s="20" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="G46" s="20"/>
       <c r="H46" s="20"/>
@@ -3354,18 +3420,18 @@
       <c r="AB46" s="3"/>
     </row>
     <row r="47" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="46"/>
-      <c r="B47" s="37"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E47" s="42"/>
-      <c r="F47" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
+      <c r="A47" s="70"/>
+      <c r="B47" s="83"/>
+      <c r="C47" s="74"/>
+      <c r="D47" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="E47" s="77"/>
+      <c r="F47" s="21">
+        <v>44740</v>
+      </c>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
       <c r="I47" s="15"/>
       <c r="J47" s="3"/>
       <c r="K47" s="3"/>
@@ -3388,15 +3454,15 @@
       <c r="AB47" s="3"/>
     </row>
     <row r="48" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="46"/>
-      <c r="B48" s="37"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E48" s="42"/>
-      <c r="F48" s="21">
-        <v>36703</v>
+      <c r="A48" s="70"/>
+      <c r="B48" s="83"/>
+      <c r="C48" s="74"/>
+      <c r="D48" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="78"/>
+      <c r="F48" s="23" t="s">
+        <v>13</v>
       </c>
       <c r="G48" s="21"/>
       <c r="H48" s="21"/>
@@ -3422,19 +3488,23 @@
       <c r="AB48" s="3"/>
     </row>
     <row r="49" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="46"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="40"/>
-      <c r="D49" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E49" s="43"/>
-      <c r="F49" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="15"/>
+      <c r="A49" s="71"/>
+      <c r="B49" s="83"/>
+      <c r="C49" s="75"/>
+      <c r="D49" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" s="80"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H49" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I49" s="19" t="s">
+        <v>6</v>
+      </c>
       <c r="J49" s="3"/>
       <c r="K49" s="3"/>
       <c r="L49" s="3"/>
@@ -3456,23 +3526,23 @@
       <c r="AB49" s="3"/>
     </row>
     <row r="50" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="47"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="41"/>
-      <c r="D50" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E50" s="44"/>
-      <c r="F50" s="24"/>
-      <c r="G50" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="H50" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I50" s="25" t="s">
-        <v>7</v>
-      </c>
+      <c r="A50" s="69" t="s">
+        <v>31</v>
+      </c>
+      <c r="B50" s="83"/>
+      <c r="C50" s="81" t="s">
+        <v>42</v>
+      </c>
+      <c r="D50" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="E50" s="77"/>
+      <c r="F50" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="G50" s="20"/>
+      <c r="H50" s="20"/>
+      <c r="I50" s="15"/>
       <c r="J50" s="3"/>
       <c r="K50" s="3"/>
       <c r="L50" s="3"/>
@@ -3494,19 +3564,15 @@
       <c r="AB50" s="3"/>
     </row>
     <row r="51" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="26" t="s">
-        <v>21</v>
-      </c>
-      <c r="B51" s="37"/>
-      <c r="C51" s="28" t="s">
-        <v>45</v>
-      </c>
-      <c r="D51" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E51" s="42"/>
+      <c r="A51" s="70"/>
+      <c r="B51" s="83"/>
+      <c r="C51" s="74"/>
+      <c r="D51" s="76" t="s">
+        <v>23</v>
+      </c>
+      <c r="E51" s="77"/>
       <c r="F51" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G51" s="20"/>
       <c r="H51" s="20"/>
@@ -3532,18 +3598,18 @@
       <c r="AB51" s="3"/>
     </row>
     <row r="52" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="46"/>
-      <c r="B52" s="37"/>
-      <c r="C52" s="51"/>
-      <c r="D52" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E52" s="42"/>
-      <c r="F52" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="G52" s="20"/>
-      <c r="H52" s="20"/>
+      <c r="A52" s="70"/>
+      <c r="B52" s="83"/>
+      <c r="C52" s="74"/>
+      <c r="D52" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" s="77"/>
+      <c r="F52" s="21">
+        <v>44741</v>
+      </c>
+      <c r="G52" s="21"/>
+      <c r="H52" s="21"/>
       <c r="I52" s="15"/>
       <c r="J52" s="3"/>
       <c r="K52" s="3"/>
@@ -3566,15 +3632,15 @@
       <c r="AB52" s="3"/>
     </row>
     <row r="53" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="46"/>
-      <c r="B53" s="37"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E53" s="42"/>
-      <c r="F53" s="21">
-        <v>44740</v>
+      <c r="A53" s="70"/>
+      <c r="B53" s="83"/>
+      <c r="C53" s="74"/>
+      <c r="D53" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="E53" s="78"/>
+      <c r="F53" s="23" t="s">
+        <v>13</v>
       </c>
       <c r="G53" s="21"/>
       <c r="H53" s="21"/>
@@ -3600,19 +3666,23 @@
       <c r="AB53" s="3"/>
     </row>
     <row r="54" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="46"/>
-      <c r="B54" s="37"/>
-      <c r="C54" s="40"/>
-      <c r="D54" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E54" s="43"/>
-      <c r="F54" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G54" s="21"/>
-      <c r="H54" s="21"/>
-      <c r="I54" s="15"/>
+      <c r="A54" s="71"/>
+      <c r="B54" s="84"/>
+      <c r="C54" s="75"/>
+      <c r="D54" s="79" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" s="80"/>
+      <c r="F54" s="24"/>
+      <c r="G54" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="H54" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="I54" s="19" t="s">
+        <v>6</v>
+      </c>
       <c r="J54" s="3"/>
       <c r="K54" s="3"/>
       <c r="L54" s="3"/>
@@ -3634,23 +3704,23 @@
       <c r="AB54" s="3"/>
     </row>
     <row r="55" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="47"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="41"/>
-      <c r="D55" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E55" s="44"/>
-      <c r="F55" s="24"/>
-      <c r="G55" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H55" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I55" s="19" t="s">
-        <v>6</v>
-      </c>
+      <c r="A55" s="69" t="s">
+        <v>32</v>
+      </c>
+      <c r="B55" s="82" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="D55" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="E55" s="100"/>
+      <c r="F55" s="20"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="20"/>
+      <c r="I55" s="15"/>
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
@@ -3672,20 +3742,14 @@
       <c r="AB55" s="3"/>
     </row>
     <row r="56" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B56" s="37"/>
-      <c r="C56" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="D56" s="31" t="s">
-        <v>22</v>
-      </c>
-      <c r="E56" s="42"/>
-      <c r="F56" s="20" t="s">
-        <v>40</v>
-      </c>
+      <c r="A56" s="69"/>
+      <c r="B56" s="83"/>
+      <c r="C56" s="113"/>
+      <c r="D56" s="76" t="s">
+        <v>35</v>
+      </c>
+      <c r="E56" s="100"/>
+      <c r="F56" s="20"/>
       <c r="G56" s="20"/>
       <c r="H56" s="20"/>
       <c r="I56" s="15"/>
@@ -3710,18 +3774,14 @@
       <c r="AB56" s="3"/>
     </row>
     <row r="57" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="46"/>
-      <c r="B57" s="37"/>
-      <c r="C57" s="40"/>
-      <c r="D57" s="31" t="s">
-        <v>23</v>
-      </c>
-      <c r="E57" s="42"/>
-      <c r="F57" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="G57" s="20"/>
-      <c r="H57" s="20"/>
+      <c r="A57" s="69"/>
+      <c r="B57" s="83"/>
+      <c r="C57" s="113"/>
+      <c r="D57" s="76"/>
+      <c r="E57" s="100"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
       <c r="I57" s="15"/>
       <c r="J57" s="3"/>
       <c r="K57" s="3"/>
@@ -3744,16 +3804,12 @@
       <c r="AB57" s="3"/>
     </row>
     <row r="58" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="46"/>
-      <c r="B58" s="37"/>
-      <c r="C58" s="40"/>
-      <c r="D58" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="E58" s="42"/>
-      <c r="F58" s="21">
-        <v>44741</v>
-      </c>
+      <c r="A58" s="69"/>
+      <c r="B58" s="83"/>
+      <c r="C58" s="113"/>
+      <c r="D58" s="76"/>
+      <c r="E58" s="96"/>
+      <c r="F58" s="23"/>
       <c r="G58" s="21"/>
       <c r="H58" s="21"/>
       <c r="I58" s="15"/>
@@ -3778,19 +3834,21 @@
       <c r="AB58" s="3"/>
     </row>
     <row r="59" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="46"/>
-      <c r="B59" s="37"/>
-      <c r="C59" s="40"/>
-      <c r="D59" s="31" t="s">
-        <v>25</v>
-      </c>
-      <c r="E59" s="43"/>
-      <c r="F59" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="G59" s="21"/>
-      <c r="H59" s="21"/>
-      <c r="I59" s="15"/>
+      <c r="A59" s="119"/>
+      <c r="B59" s="84"/>
+      <c r="C59" s="114"/>
+      <c r="D59" s="79"/>
+      <c r="E59" s="120"/>
+      <c r="F59" s="24"/>
+      <c r="G59" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="H59" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I59" s="19" t="s">
+        <v>6</v>
+      </c>
       <c r="J59" s="3"/>
       <c r="K59" s="3"/>
       <c r="L59" s="3"/>
@@ -3812,23 +3870,15 @@
       <c r="AB59" s="3"/>
     </row>
     <row r="60" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="47"/>
-      <c r="B60" s="38"/>
-      <c r="C60" s="41"/>
-      <c r="D60" s="34" t="s">
-        <v>28</v>
-      </c>
-      <c r="E60" s="44"/>
-      <c r="F60" s="24"/>
-      <c r="G60" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="H60" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="I60" s="19" t="s">
-        <v>6</v>
-      </c>
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="3"/>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="3"/>
+      <c r="I60" s="3"/>
       <c r="J60" s="3"/>
       <c r="K60" s="3"/>
       <c r="L60" s="3"/>
@@ -3850,23 +3900,15 @@
       <c r="AB60" s="3"/>
     </row>
     <row r="61" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="26" t="s">
-        <v>32</v>
-      </c>
-      <c r="B61" s="36" t="s">
-        <v>33</v>
-      </c>
-      <c r="C61" s="28" t="s">
-        <v>37</v>
-      </c>
-      <c r="D61" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="E61" s="32"/>
-      <c r="F61" s="20"/>
-      <c r="G61" s="20"/>
-      <c r="H61" s="20"/>
-      <c r="I61" s="15"/>
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="3"/>
+      <c r="D61" s="3"/>
+      <c r="E61" s="3"/>
+      <c r="F61" s="3"/>
+      <c r="G61" s="3"/>
+      <c r="H61" s="3"/>
+      <c r="I61" s="3"/>
       <c r="J61" s="3"/>
       <c r="K61" s="3"/>
       <c r="L61" s="3"/>
@@ -3888,17 +3930,15 @@
       <c r="AB61" s="3"/>
     </row>
     <row r="62" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="26"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="29"/>
-      <c r="D62" s="31" t="s">
-        <v>35</v>
-      </c>
-      <c r="E62" s="32"/>
-      <c r="F62" s="20"/>
-      <c r="G62" s="20"/>
-      <c r="H62" s="20"/>
-      <c r="I62" s="15"/>
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3"/>
+      <c r="G62" s="3"/>
+      <c r="H62" s="3"/>
+      <c r="I62" s="3"/>
       <c r="J62" s="3"/>
       <c r="K62" s="3"/>
       <c r="L62" s="3"/>
@@ -3920,15 +3960,15 @@
       <c r="AB62" s="3"/>
     </row>
     <row r="63" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="26"/>
-      <c r="B63" s="37"/>
-      <c r="C63" s="29"/>
-      <c r="D63" s="31"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="21"/>
-      <c r="G63" s="21"/>
-      <c r="H63" s="21"/>
-      <c r="I63" s="15"/>
+      <c r="A63" s="3"/>
+      <c r="B63" s="3"/>
+      <c r="C63" s="3"/>
+      <c r="D63" s="3"/>
+      <c r="E63" s="3"/>
+      <c r="F63" s="3"/>
+      <c r="G63" s="3"/>
+      <c r="H63" s="3"/>
+      <c r="I63" s="3"/>
       <c r="J63" s="3"/>
       <c r="K63" s="3"/>
       <c r="L63" s="3"/>
@@ -3950,15 +3990,15 @@
       <c r="AB63" s="3"/>
     </row>
     <row r="64" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="26"/>
-      <c r="B64" s="37"/>
-      <c r="C64" s="29"/>
-      <c r="D64" s="31"/>
-      <c r="E64" s="33"/>
-      <c r="F64" s="23"/>
-      <c r="G64" s="21"/>
-      <c r="H64" s="21"/>
-      <c r="I64" s="15"/>
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
+      <c r="C64" s="3"/>
+      <c r="D64" s="3"/>
+      <c r="E64" s="3"/>
+      <c r="F64" s="3"/>
+      <c r="G64" s="3"/>
+      <c r="H64" s="3"/>
+      <c r="I64" s="3"/>
       <c r="J64" s="3"/>
       <c r="K64" s="3"/>
       <c r="L64" s="3"/>
@@ -3980,21 +4020,15 @@
       <c r="AB64" s="3"/>
     </row>
     <row r="65" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="27"/>
-      <c r="B65" s="38"/>
-      <c r="C65" s="30"/>
-      <c r="D65" s="34"/>
-      <c r="E65" s="35"/>
-      <c r="F65" s="24"/>
-      <c r="G65" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="H65" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="I65" s="19" t="s">
-        <v>6</v>
-      </c>
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="3"/>
+      <c r="D65" s="3"/>
+      <c r="E65" s="3"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="3"/>
+      <c r="H65" s="3"/>
+      <c r="I65" s="3"/>
       <c r="J65" s="3"/>
       <c r="K65" s="3"/>
       <c r="L65" s="3"/>
@@ -4016,15 +4050,6 @@
       <c r="AB65" s="3"/>
     </row>
     <row r="66" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="3"/>
-      <c r="B66" s="3"/>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="3"/>
       <c r="J66" s="3"/>
       <c r="K66" s="3"/>
       <c r="L66" s="3"/>
@@ -4046,15 +4071,6 @@
       <c r="AB66" s="3"/>
     </row>
     <row r="67" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="3"/>
-      <c r="B67" s="3"/>
-      <c r="C67" s="3"/>
-      <c r="D67" s="3"/>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3"/>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3"/>
-      <c r="I67" s="3"/>
       <c r="J67" s="3"/>
       <c r="K67" s="3"/>
       <c r="L67" s="3"/>
@@ -4076,15 +4092,6 @@
       <c r="AB67" s="3"/>
     </row>
     <row r="68" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="3"/>
-      <c r="B68" s="3"/>
-      <c r="C68" s="3"/>
-      <c r="D68" s="3"/>
-      <c r="E68" s="3"/>
-      <c r="F68" s="3"/>
-      <c r="G68" s="3"/>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3"/>
       <c r="J68" s="3"/>
       <c r="K68" s="3"/>
       <c r="L68" s="3"/>
@@ -4106,15 +4113,6 @@
       <c r="AB68" s="3"/>
     </row>
     <row r="69" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="3"/>
-      <c r="B69" s="3"/>
-      <c r="C69" s="3"/>
-      <c r="D69" s="3"/>
-      <c r="E69" s="3"/>
-      <c r="F69" s="3"/>
-      <c r="G69" s="3"/>
-      <c r="H69" s="3"/>
-      <c r="I69" s="3"/>
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
@@ -4136,15 +4134,6 @@
       <c r="AB69" s="3"/>
     </row>
     <row r="70" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="3"/>
-      <c r="B70" s="3"/>
-      <c r="C70" s="3"/>
-      <c r="D70" s="3"/>
-      <c r="E70" s="3"/>
-      <c r="F70" s="3"/>
-      <c r="G70" s="3"/>
-      <c r="H70" s="3"/>
-      <c r="I70" s="3"/>
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
@@ -4196,6 +4185,15 @@
       <c r="AB71" s="3"/>
     </row>
     <row r="72" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="3"/>
+      <c r="B72" s="3"/>
+      <c r="C72" s="3"/>
+      <c r="D72" s="3"/>
+      <c r="E72" s="3"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="3"/>
+      <c r="H72" s="3"/>
+      <c r="I72" s="3"/>
       <c r="J72" s="3"/>
       <c r="K72" s="3"/>
       <c r="L72" s="3"/>
@@ -4217,6 +4215,15 @@
       <c r="AB72" s="3"/>
     </row>
     <row r="73" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="3"/>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+      <c r="D73" s="3"/>
+      <c r="E73" s="3"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="3"/>
+      <c r="H73" s="3"/>
+      <c r="I73" s="3"/>
       <c r="J73" s="3"/>
       <c r="K73" s="3"/>
       <c r="L73" s="3"/>
@@ -4238,6 +4245,15 @@
       <c r="AB73" s="3"/>
     </row>
     <row r="74" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="3"/>
+      <c r="B74" s="3"/>
+      <c r="C74" s="3"/>
+      <c r="D74" s="3"/>
+      <c r="E74" s="3"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="3"/>
+      <c r="H74" s="3"/>
+      <c r="I74" s="3"/>
       <c r="J74" s="3"/>
       <c r="K74" s="3"/>
       <c r="L74" s="3"/>
@@ -4259,6 +4275,15 @@
       <c r="AB74" s="3"/>
     </row>
     <row r="75" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="3"/>
+      <c r="B75" s="3"/>
+      <c r="C75" s="3"/>
+      <c r="D75" s="3"/>
+      <c r="E75" s="3"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="3"/>
+      <c r="H75" s="3"/>
+      <c r="I75" s="3"/>
       <c r="J75" s="3"/>
       <c r="K75" s="3"/>
       <c r="L75" s="3"/>
@@ -4280,6 +4305,15 @@
       <c r="AB75" s="3"/>
     </row>
     <row r="76" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="3"/>
+      <c r="B76" s="3"/>
+      <c r="C76" s="3"/>
+      <c r="D76" s="3"/>
+      <c r="E76" s="3"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="3"/>
+      <c r="H76" s="3"/>
+      <c r="I76" s="3"/>
       <c r="J76" s="3"/>
       <c r="K76" s="3"/>
       <c r="L76" s="3"/>
@@ -8470,185 +8504,185 @@
       <c r="AA215" s="3"/>
       <c r="AB215" s="3"/>
     </row>
-    <row r="216" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A216" s="3"/>
-      <c r="B216" s="3"/>
-      <c r="C216" s="3"/>
-      <c r="D216" s="3"/>
-      <c r="E216" s="3"/>
-      <c r="F216" s="3"/>
-      <c r="G216" s="3"/>
-      <c r="H216" s="3"/>
-      <c r="I216" s="3"/>
-      <c r="J216" s="3"/>
-      <c r="K216" s="3"/>
-      <c r="L216" s="3"/>
-      <c r="M216" s="3"/>
-      <c r="N216" s="3"/>
-      <c r="O216" s="3"/>
-      <c r="P216" s="3"/>
-      <c r="Q216" s="3"/>
-      <c r="R216" s="3"/>
-      <c r="S216" s="3"/>
-      <c r="T216" s="3"/>
-      <c r="U216" s="3"/>
-      <c r="V216" s="3"/>
-      <c r="W216" s="3"/>
-      <c r="X216" s="3"/>
-      <c r="Y216" s="3"/>
-      <c r="Z216" s="3"/>
-      <c r="AA216" s="3"/>
-      <c r="AB216" s="3"/>
-    </row>
-    <row r="217" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A217" s="3"/>
-      <c r="B217" s="3"/>
-      <c r="C217" s="3"/>
-      <c r="D217" s="3"/>
-      <c r="E217" s="3"/>
-      <c r="F217" s="3"/>
-      <c r="G217" s="3"/>
-      <c r="H217" s="3"/>
-      <c r="I217" s="3"/>
-      <c r="J217" s="3"/>
-      <c r="K217" s="3"/>
-      <c r="L217" s="3"/>
-      <c r="M217" s="3"/>
-      <c r="N217" s="3"/>
-      <c r="O217" s="3"/>
-      <c r="P217" s="3"/>
-      <c r="Q217" s="3"/>
-      <c r="R217" s="3"/>
-      <c r="S217" s="3"/>
-      <c r="T217" s="3"/>
-      <c r="U217" s="3"/>
-      <c r="V217" s="3"/>
-      <c r="W217" s="3"/>
-      <c r="X217" s="3"/>
-      <c r="Y217" s="3"/>
-      <c r="Z217" s="3"/>
-      <c r="AA217" s="3"/>
-      <c r="AB217" s="3"/>
-    </row>
-    <row r="218" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A218" s="3"/>
-      <c r="B218" s="3"/>
-      <c r="C218" s="3"/>
-      <c r="D218" s="3"/>
-      <c r="E218" s="3"/>
-      <c r="F218" s="3"/>
-      <c r="G218" s="3"/>
-      <c r="H218" s="3"/>
-      <c r="I218" s="3"/>
-      <c r="J218" s="3"/>
-      <c r="K218" s="3"/>
-      <c r="L218" s="3"/>
-      <c r="M218" s="3"/>
-      <c r="N218" s="3"/>
-      <c r="O218" s="3"/>
-      <c r="P218" s="3"/>
-      <c r="Q218" s="3"/>
-      <c r="R218" s="3"/>
-      <c r="S218" s="3"/>
-      <c r="T218" s="3"/>
-      <c r="U218" s="3"/>
-      <c r="V218" s="3"/>
-      <c r="W218" s="3"/>
-      <c r="X218" s="3"/>
-      <c r="Y218" s="3"/>
-      <c r="Z218" s="3"/>
-      <c r="AA218" s="3"/>
-      <c r="AB218" s="3"/>
-    </row>
-    <row r="219" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A219" s="3"/>
-      <c r="B219" s="3"/>
-      <c r="C219" s="3"/>
-      <c r="D219" s="3"/>
-      <c r="E219" s="3"/>
-      <c r="F219" s="3"/>
-      <c r="G219" s="3"/>
-      <c r="H219" s="3"/>
-      <c r="I219" s="3"/>
-      <c r="J219" s="3"/>
-      <c r="K219" s="3"/>
-      <c r="L219" s="3"/>
-      <c r="M219" s="3"/>
-      <c r="N219" s="3"/>
-      <c r="O219" s="3"/>
-      <c r="P219" s="3"/>
-      <c r="Q219" s="3"/>
-      <c r="R219" s="3"/>
-      <c r="S219" s="3"/>
-      <c r="T219" s="3"/>
-      <c r="U219" s="3"/>
-      <c r="V219" s="3"/>
-      <c r="W219" s="3"/>
-      <c r="X219" s="3"/>
-      <c r="Y219" s="3"/>
-      <c r="Z219" s="3"/>
-      <c r="AA219" s="3"/>
-      <c r="AB219" s="3"/>
-    </row>
-    <row r="220" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A220" s="3"/>
-      <c r="B220" s="3"/>
-      <c r="C220" s="3"/>
-      <c r="D220" s="3"/>
-      <c r="E220" s="3"/>
-      <c r="F220" s="3"/>
-      <c r="G220" s="3"/>
-      <c r="H220" s="3"/>
-      <c r="I220" s="3"/>
-      <c r="J220" s="3"/>
-      <c r="K220" s="3"/>
-      <c r="L220" s="3"/>
-      <c r="M220" s="3"/>
-      <c r="N220" s="3"/>
-      <c r="O220" s="3"/>
-      <c r="P220" s="3"/>
-      <c r="Q220" s="3"/>
-      <c r="R220" s="3"/>
-      <c r="S220" s="3"/>
-      <c r="T220" s="3"/>
-      <c r="U220" s="3"/>
-      <c r="V220" s="3"/>
-      <c r="W220" s="3"/>
-      <c r="X220" s="3"/>
-      <c r="Y220" s="3"/>
-      <c r="Z220" s="3"/>
-      <c r="AA220" s="3"/>
-      <c r="AB220" s="3"/>
-    </row>
-    <row r="221" spans="1:28" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A221" s="3"/>
-      <c r="B221" s="3"/>
-      <c r="C221" s="3"/>
-      <c r="D221" s="3"/>
-      <c r="E221" s="3"/>
-      <c r="F221" s="3"/>
-      <c r="G221" s="3"/>
-      <c r="H221" s="3"/>
-      <c r="I221" s="3"/>
-      <c r="J221" s="3"/>
-      <c r="K221" s="3"/>
-      <c r="L221" s="3"/>
-      <c r="M221" s="3"/>
-      <c r="N221" s="3"/>
-      <c r="O221" s="3"/>
-      <c r="P221" s="3"/>
-      <c r="Q221" s="3"/>
-      <c r="R221" s="3"/>
-      <c r="S221" s="3"/>
-      <c r="T221" s="3"/>
-      <c r="U221" s="3"/>
-      <c r="V221" s="3"/>
-      <c r="W221" s="3"/>
-      <c r="X221" s="3"/>
-      <c r="Y221" s="3"/>
-      <c r="Z221" s="3"/>
-      <c r="AA221" s="3"/>
-      <c r="AB221" s="3"/>
+    <row r="216" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A216" s="2"/>
+      <c r="B216" s="2"/>
+      <c r="C216" s="2"/>
+      <c r="D216" s="2"/>
+      <c r="E216" s="2"/>
+      <c r="F216" s="2"/>
+      <c r="G216" s="2"/>
+      <c r="H216" s="2"/>
+      <c r="I216" s="2"/>
+      <c r="J216" s="2"/>
+      <c r="K216" s="2"/>
+      <c r="L216" s="2"/>
+      <c r="M216" s="2"/>
+      <c r="N216" s="2"/>
+      <c r="O216" s="2"/>
+      <c r="P216" s="2"/>
+      <c r="Q216" s="2"/>
+      <c r="R216" s="2"/>
+      <c r="S216" s="2"/>
+      <c r="T216" s="2"/>
+      <c r="U216" s="2"/>
+      <c r="V216" s="2"/>
+      <c r="W216" s="2"/>
+      <c r="X216" s="2"/>
+      <c r="Y216" s="2"/>
+      <c r="Z216" s="2"/>
+      <c r="AA216" s="2"/>
+      <c r="AB216" s="2"/>
+    </row>
+    <row r="217" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A217" s="2"/>
+      <c r="B217" s="2"/>
+      <c r="C217" s="2"/>
+      <c r="D217" s="2"/>
+      <c r="E217" s="2"/>
+      <c r="F217" s="2"/>
+      <c r="G217" s="2"/>
+      <c r="H217" s="2"/>
+      <c r="I217" s="2"/>
+      <c r="J217" s="2"/>
+      <c r="K217" s="2"/>
+      <c r="L217" s="2"/>
+      <c r="M217" s="2"/>
+      <c r="N217" s="2"/>
+      <c r="O217" s="2"/>
+      <c r="P217" s="2"/>
+      <c r="Q217" s="2"/>
+      <c r="R217" s="2"/>
+      <c r="S217" s="2"/>
+      <c r="T217" s="2"/>
+      <c r="U217" s="2"/>
+      <c r="V217" s="2"/>
+      <c r="W217" s="2"/>
+      <c r="X217" s="2"/>
+      <c r="Y217" s="2"/>
+      <c r="Z217" s="2"/>
+      <c r="AA217" s="2"/>
+      <c r="AB217" s="2"/>
+    </row>
+    <row r="218" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A218" s="2"/>
+      <c r="B218" s="2"/>
+      <c r="C218" s="2"/>
+      <c r="D218" s="2"/>
+      <c r="E218" s="2"/>
+      <c r="F218" s="2"/>
+      <c r="G218" s="2"/>
+      <c r="H218" s="2"/>
+      <c r="I218" s="2"/>
+      <c r="J218" s="2"/>
+      <c r="K218" s="2"/>
+      <c r="L218" s="2"/>
+      <c r="M218" s="2"/>
+      <c r="N218" s="2"/>
+      <c r="O218" s="2"/>
+      <c r="P218" s="2"/>
+      <c r="Q218" s="2"/>
+      <c r="R218" s="2"/>
+      <c r="S218" s="2"/>
+      <c r="T218" s="2"/>
+      <c r="U218" s="2"/>
+      <c r="V218" s="2"/>
+      <c r="W218" s="2"/>
+      <c r="X218" s="2"/>
+      <c r="Y218" s="2"/>
+      <c r="Z218" s="2"/>
+      <c r="AA218" s="2"/>
+      <c r="AB218" s="2"/>
+    </row>
+    <row r="219" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A219" s="2"/>
+      <c r="B219" s="2"/>
+      <c r="C219" s="2"/>
+      <c r="D219" s="2"/>
+      <c r="E219" s="2"/>
+      <c r="F219" s="2"/>
+      <c r="G219" s="2"/>
+      <c r="H219" s="2"/>
+      <c r="I219" s="2"/>
+      <c r="J219" s="2"/>
+      <c r="K219" s="2"/>
+      <c r="L219" s="2"/>
+      <c r="M219" s="2"/>
+      <c r="N219" s="2"/>
+      <c r="O219" s="2"/>
+      <c r="P219" s="2"/>
+      <c r="Q219" s="2"/>
+      <c r="R219" s="2"/>
+      <c r="S219" s="2"/>
+      <c r="T219" s="2"/>
+      <c r="U219" s="2"/>
+      <c r="V219" s="2"/>
+      <c r="W219" s="2"/>
+      <c r="X219" s="2"/>
+      <c r="Y219" s="2"/>
+      <c r="Z219" s="2"/>
+      <c r="AA219" s="2"/>
+      <c r="AB219" s="2"/>
+    </row>
+    <row r="220" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A220" s="2"/>
+      <c r="B220" s="2"/>
+      <c r="C220" s="2"/>
+      <c r="D220" s="2"/>
+      <c r="E220" s="2"/>
+      <c r="F220" s="2"/>
+      <c r="G220" s="2"/>
+      <c r="H220" s="2"/>
+      <c r="I220" s="2"/>
+      <c r="J220" s="2"/>
+      <c r="K220" s="2"/>
+      <c r="L220" s="2"/>
+      <c r="M220" s="2"/>
+      <c r="N220" s="2"/>
+      <c r="O220" s="2"/>
+      <c r="P220" s="2"/>
+      <c r="Q220" s="2"/>
+      <c r="R220" s="2"/>
+      <c r="S220" s="2"/>
+      <c r="T220" s="2"/>
+      <c r="U220" s="2"/>
+      <c r="V220" s="2"/>
+      <c r="W220" s="2"/>
+      <c r="X220" s="2"/>
+      <c r="Y220" s="2"/>
+      <c r="Z220" s="2"/>
+      <c r="AA220" s="2"/>
+      <c r="AB220" s="2"/>
+    </row>
+    <row r="221" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A221" s="2"/>
+      <c r="B221" s="2"/>
+      <c r="C221" s="2"/>
+      <c r="D221" s="2"/>
+      <c r="E221" s="2"/>
+      <c r="F221" s="2"/>
+      <c r="G221" s="2"/>
+      <c r="H221" s="2"/>
+      <c r="I221" s="2"/>
+      <c r="J221" s="2"/>
+      <c r="K221" s="2"/>
+      <c r="L221" s="2"/>
+      <c r="M221" s="2"/>
+      <c r="N221" s="2"/>
+      <c r="O221" s="2"/>
+      <c r="P221" s="2"/>
+      <c r="Q221" s="2"/>
+      <c r="R221" s="2"/>
+      <c r="S221" s="2"/>
+      <c r="T221" s="2"/>
+      <c r="U221" s="2"/>
+      <c r="V221" s="2"/>
+      <c r="W221" s="2"/>
+      <c r="X221" s="2"/>
+      <c r="Y221" s="2"/>
+      <c r="Z221" s="2"/>
+      <c r="AA221" s="2"/>
+      <c r="AB221" s="2"/>
     </row>
     <row r="222" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="2"/>
@@ -8710,197 +8744,23 @@
       <c r="AA223" s="2"/>
       <c r="AB223" s="2"/>
     </row>
-    <row r="224" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A224" s="2"/>
-      <c r="B224" s="2"/>
-      <c r="C224" s="2"/>
-      <c r="D224" s="2"/>
-      <c r="E224" s="2"/>
-      <c r="F224" s="2"/>
-      <c r="G224" s="2"/>
-      <c r="H224" s="2"/>
-      <c r="I224" s="2"/>
-      <c r="J224" s="2"/>
-      <c r="K224" s="2"/>
-      <c r="L224" s="2"/>
-      <c r="M224" s="2"/>
-      <c r="N224" s="2"/>
-      <c r="O224" s="2"/>
-      <c r="P224" s="2"/>
-      <c r="Q224" s="2"/>
-      <c r="R224" s="2"/>
-      <c r="S224" s="2"/>
-      <c r="T224" s="2"/>
-      <c r="U224" s="2"/>
-      <c r="V224" s="2"/>
-      <c r="W224" s="2"/>
-      <c r="X224" s="2"/>
-      <c r="Y224" s="2"/>
-      <c r="Z224" s="2"/>
-      <c r="AA224" s="2"/>
-      <c r="AB224" s="2"/>
-    </row>
-    <row r="225" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A225" s="2"/>
-      <c r="B225" s="2"/>
-      <c r="C225" s="2"/>
-      <c r="D225" s="2"/>
-      <c r="E225" s="2"/>
-      <c r="F225" s="2"/>
-      <c r="G225" s="2"/>
-      <c r="H225" s="2"/>
-      <c r="I225" s="2"/>
-      <c r="J225" s="2"/>
-      <c r="K225" s="2"/>
-      <c r="L225" s="2"/>
-      <c r="M225" s="2"/>
-      <c r="N225" s="2"/>
-      <c r="O225" s="2"/>
-      <c r="P225" s="2"/>
-      <c r="Q225" s="2"/>
-      <c r="R225" s="2"/>
-      <c r="S225" s="2"/>
-      <c r="T225" s="2"/>
-      <c r="U225" s="2"/>
-      <c r="V225" s="2"/>
-      <c r="W225" s="2"/>
-      <c r="X225" s="2"/>
-      <c r="Y225" s="2"/>
-      <c r="Z225" s="2"/>
-      <c r="AA225" s="2"/>
-      <c r="AB225" s="2"/>
-    </row>
-    <row r="226" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A226" s="2"/>
-      <c r="B226" s="2"/>
-      <c r="C226" s="2"/>
-      <c r="D226" s="2"/>
-      <c r="E226" s="2"/>
-      <c r="F226" s="2"/>
-      <c r="G226" s="2"/>
-      <c r="H226" s="2"/>
-      <c r="I226" s="2"/>
-      <c r="J226" s="2"/>
-      <c r="K226" s="2"/>
-      <c r="L226" s="2"/>
-      <c r="M226" s="2"/>
-      <c r="N226" s="2"/>
-      <c r="O226" s="2"/>
-      <c r="P226" s="2"/>
-      <c r="Q226" s="2"/>
-      <c r="R226" s="2"/>
-      <c r="S226" s="2"/>
-      <c r="T226" s="2"/>
-      <c r="U226" s="2"/>
-      <c r="V226" s="2"/>
-      <c r="W226" s="2"/>
-      <c r="X226" s="2"/>
-      <c r="Y226" s="2"/>
-      <c r="Z226" s="2"/>
-      <c r="AA226" s="2"/>
-      <c r="AB226" s="2"/>
-    </row>
-    <row r="227" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A227" s="2"/>
-      <c r="B227" s="2"/>
-      <c r="C227" s="2"/>
-      <c r="D227" s="2"/>
-      <c r="E227" s="2"/>
-      <c r="F227" s="2"/>
-      <c r="G227" s="2"/>
-      <c r="H227" s="2"/>
-      <c r="I227" s="2"/>
-      <c r="J227" s="2"/>
-      <c r="K227" s="2"/>
-      <c r="L227" s="2"/>
-      <c r="M227" s="2"/>
-      <c r="N227" s="2"/>
-      <c r="O227" s="2"/>
-      <c r="P227" s="2"/>
-      <c r="Q227" s="2"/>
-      <c r="R227" s="2"/>
-      <c r="S227" s="2"/>
-      <c r="T227" s="2"/>
-      <c r="U227" s="2"/>
-      <c r="V227" s="2"/>
-      <c r="W227" s="2"/>
-      <c r="X227" s="2"/>
-      <c r="Y227" s="2"/>
-      <c r="Z227" s="2"/>
-      <c r="AA227" s="2"/>
-      <c r="AB227" s="2"/>
-    </row>
-    <row r="228" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A228" s="2"/>
-      <c r="B228" s="2"/>
-      <c r="C228" s="2"/>
-      <c r="D228" s="2"/>
-      <c r="E228" s="2"/>
-      <c r="F228" s="2"/>
-      <c r="G228" s="2"/>
-      <c r="H228" s="2"/>
-      <c r="I228" s="2"/>
-      <c r="J228" s="2"/>
-      <c r="K228" s="2"/>
-      <c r="L228" s="2"/>
-      <c r="M228" s="2"/>
-      <c r="N228" s="2"/>
-      <c r="O228" s="2"/>
-      <c r="P228" s="2"/>
-      <c r="Q228" s="2"/>
-      <c r="R228" s="2"/>
-      <c r="S228" s="2"/>
-      <c r="T228" s="2"/>
-      <c r="U228" s="2"/>
-      <c r="V228" s="2"/>
-      <c r="W228" s="2"/>
-      <c r="X228" s="2"/>
-      <c r="Y228" s="2"/>
-      <c r="Z228" s="2"/>
-      <c r="AA228" s="2"/>
-      <c r="AB228" s="2"/>
-    </row>
-    <row r="229" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A229" s="2"/>
-      <c r="B229" s="2"/>
-      <c r="C229" s="2"/>
-      <c r="D229" s="2"/>
-      <c r="E229" s="2"/>
-      <c r="F229" s="2"/>
-      <c r="G229" s="2"/>
-      <c r="H229" s="2"/>
-      <c r="I229" s="2"/>
-      <c r="J229" s="2"/>
-      <c r="K229" s="2"/>
-      <c r="L229" s="2"/>
-      <c r="M229" s="2"/>
-      <c r="N229" s="2"/>
-      <c r="O229" s="2"/>
-      <c r="P229" s="2"/>
-      <c r="Q229" s="2"/>
-      <c r="R229" s="2"/>
-      <c r="S229" s="2"/>
-      <c r="T229" s="2"/>
-      <c r="U229" s="2"/>
-      <c r="V229" s="2"/>
-      <c r="W229" s="2"/>
-      <c r="X229" s="2"/>
-      <c r="Y229" s="2"/>
-      <c r="Z229" s="2"/>
-      <c r="AA229" s="2"/>
-      <c r="AB229" s="2"/>
-    </row>
-    <row r="230" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" spans="1:28" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -9664,20 +9524,83 @@
     <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1002" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1003" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1004" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1005" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1006" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1007" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1008" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="97">
-    <mergeCell ref="B21:B32"/>
-    <mergeCell ref="C13:C16"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="D15:E15"/>
-    <mergeCell ref="D16:E16"/>
+  <mergeCells count="89">
+    <mergeCell ref="A55:A59"/>
+    <mergeCell ref="C55:C59"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="D59:E59"/>
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="C40:C44"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="D41:E41"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="D33:E33"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="C27:C30"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="D23:E23"/>
+    <mergeCell ref="D24:E24"/>
+    <mergeCell ref="C21:C23"/>
+    <mergeCell ref="C31:C34"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="D26:E26"/>
+    <mergeCell ref="D34:E34"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="B27:B34"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="D22:E22"/>
+    <mergeCell ref="D29:E29"/>
+    <mergeCell ref="D30:E30"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="E3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="D27:E27"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="C9:C12"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A50:A54"/>
+    <mergeCell ref="C50:C54"/>
+    <mergeCell ref="D50:E50"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E54"/>
+    <mergeCell ref="B35:B54"/>
+    <mergeCell ref="A35:A39"/>
+    <mergeCell ref="C35:C39"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="D36:E36"/>
+    <mergeCell ref="D37:E37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A40:A44"/>
+    <mergeCell ref="A45:A49"/>
+    <mergeCell ref="C45:C49"/>
+    <mergeCell ref="D45:E45"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="D47:E47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="D49:E49"/>
     <mergeCell ref="A17:A20"/>
     <mergeCell ref="B9:B20"/>
     <mergeCell ref="D17:E17"/>
@@ -9686,89 +9609,12 @@
     <mergeCell ref="D20:E20"/>
     <mergeCell ref="C17:C20"/>
     <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A51:A55"/>
-    <mergeCell ref="C51:C55"/>
-    <mergeCell ref="D51:E51"/>
-    <mergeCell ref="D52:E52"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E54"/>
-    <mergeCell ref="D55:E55"/>
-    <mergeCell ref="A56:A60"/>
-    <mergeCell ref="C56:C60"/>
-    <mergeCell ref="D56:E56"/>
-    <mergeCell ref="D57:E57"/>
-    <mergeCell ref="D58:E58"/>
-    <mergeCell ref="D59:E59"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="B41:B60"/>
-    <mergeCell ref="A41:A45"/>
-    <mergeCell ref="C41:C45"/>
-    <mergeCell ref="D41:E41"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="A46:A50"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="E3:F3"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="D33:E33"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="C9:C12"/>
-    <mergeCell ref="C29:C32"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D29:E29"/>
-    <mergeCell ref="D34:E34"/>
-    <mergeCell ref="A37:A40"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="C25:C28"/>
-    <mergeCell ref="D28:E28"/>
-    <mergeCell ref="B33:B40"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D22:E22"/>
-    <mergeCell ref="D35:E35"/>
-    <mergeCell ref="D36:E36"/>
-    <mergeCell ref="D37:E37"/>
-    <mergeCell ref="D30:E30"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A33:A36"/>
-    <mergeCell ref="C33:C36"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="D23:E23"/>
-    <mergeCell ref="D24:E24"/>
-    <mergeCell ref="C21:C24"/>
-    <mergeCell ref="C37:C40"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D26:E26"/>
-    <mergeCell ref="D27:E27"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="A25:A28"/>
-    <mergeCell ref="C46:C50"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D47:E47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="A61:A65"/>
-    <mergeCell ref="C61:C65"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="B61:B65"/>
+    <mergeCell ref="B21:B26"/>
+    <mergeCell ref="C13:C16"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="D15:E15"/>
+    <mergeCell ref="D16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>